<commit_message>
Updated Control Table uploads to include MSRP_VERSION column.
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA_Choice.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA_Choice.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gu1xkaz\IdeaProjects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>PRODUCTCD</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>SYMBOL_2000_CHOICE_T</t>
+  </si>
+  <si>
+    <t>MSRP_2000_CHOICE</t>
+  </si>
+  <si>
+    <t>MSRP_2000_CHOICE_T</t>
+  </si>
+  <si>
+    <t>MSRP_VERSION</t>
   </si>
 </sst>
 </file>
@@ -399,22 +408,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,8 +443,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -453,8 +466,11 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -472,6 +488,9 @@
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renewal, Using Oldest Entry Date case added.
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA_Choice.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA_Choice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gu1xkaz\IdeaProjects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>PRODUCTCD</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>SYMBOL_2000_CHOICE_T</t>
+  </si>
+  <si>
+    <t>SYMBOL_2000_ENTRY_DATE</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,6 +477,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>20000102</v>
+      </c>
+      <c r="E4" s="3">
+        <v>20300102</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Using Oldest moved to NB, Endorsement case added.
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA_Choice.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA_Choice.xlsx
@@ -59,7 +59,7 @@
     <t>SYMBOL_2000_CHOICE_T</t>
   </si>
   <si>
-    <t>SYMBOL_2000_ENTRY_DATE</t>
+    <t>SYMBOL_2000_CH_ENTRY_DATE</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,7 +414,7 @@
     <col min="3" max="3" width="13.21875" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>